<commit_message>
Add data type parsers.
</commit_message>
<xml_diff>
--- a/Data/TestData.xlsx
+++ b/Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13125"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <t>id</t>
   </si>
   <si>
-    <t>testBool</t>
+    <t>testBoolean</t>
   </si>
   <si>
     <t>testByte</t>
@@ -57,43 +57,43 @@
     <t>testString</t>
   </si>
   <si>
-    <t>testBoolList</t>
-  </si>
-  <si>
-    <t>testByteList</t>
-  </si>
-  <si>
-    <t>testSByteList</t>
-  </si>
-  <si>
-    <t>testShortList</t>
-  </si>
-  <si>
-    <t>testUShortList</t>
-  </si>
-  <si>
-    <t>testIntList</t>
-  </si>
-  <si>
-    <t>testUIntList</t>
-  </si>
-  <si>
-    <t>testLongList</t>
-  </si>
-  <si>
-    <t>testULongList</t>
-  </si>
-  <si>
-    <t>testFloatList</t>
-  </si>
-  <si>
-    <t>testDoubleList</t>
-  </si>
-  <si>
-    <t>testDecimalList</t>
-  </si>
-  <si>
-    <t>testStringList</t>
+    <t>testBooleanArray</t>
+  </si>
+  <si>
+    <t>testByteArray</t>
+  </si>
+  <si>
+    <t>testSByteArray</t>
+  </si>
+  <si>
+    <t>testShortArray</t>
+  </si>
+  <si>
+    <t>testUShortArray</t>
+  </si>
+  <si>
+    <t>testIntArray</t>
+  </si>
+  <si>
+    <t>testUIntArray</t>
+  </si>
+  <si>
+    <t>testLongArray</t>
+  </si>
+  <si>
+    <t>testULongArray</t>
+  </si>
+  <si>
+    <t>testFloatArray</t>
+  </si>
+  <si>
+    <t>testDoubleArray</t>
+  </si>
+  <si>
+    <t>testDecimalArray</t>
+  </si>
+  <si>
+    <t>testStringArray</t>
   </si>
   <si>
     <t>long</t>
@@ -135,43 +135,43 @@
     <t>string</t>
   </si>
   <si>
-    <t>boolList</t>
-  </si>
-  <si>
-    <t>byteList</t>
-  </si>
-  <si>
-    <t>sbyteList</t>
-  </si>
-  <si>
-    <t>shortList</t>
-  </si>
-  <si>
-    <t>ushortList</t>
-  </si>
-  <si>
-    <t>intList</t>
-  </si>
-  <si>
-    <t>uintList</t>
-  </si>
-  <si>
-    <t>longList</t>
-  </si>
-  <si>
-    <t>ulongList</t>
-  </si>
-  <si>
-    <t>floatList</t>
-  </si>
-  <si>
-    <t>doubleList</t>
-  </si>
-  <si>
-    <t>decimalList</t>
-  </si>
-  <si>
-    <t>stringList</t>
+    <t>bool[]</t>
+  </si>
+  <si>
+    <t>byte[]</t>
+  </si>
+  <si>
+    <t>sbyte[]</t>
+  </si>
+  <si>
+    <t>short[]</t>
+  </si>
+  <si>
+    <t>ushort[]</t>
+  </si>
+  <si>
+    <t>int[]</t>
+  </si>
+  <si>
+    <t>uint[]</t>
+  </si>
+  <si>
+    <t>long[]</t>
+  </si>
+  <si>
+    <t>ulong[]</t>
+  </si>
+  <si>
+    <t>float[]</t>
+  </si>
+  <si>
+    <t>double[]</t>
+  </si>
+  <si>
+    <t>decimal[]</t>
+  </si>
+  <si>
+    <t>string[]</t>
   </si>
   <si>
     <t>ID</t>
@@ -214,43 +214,43 @@
     <t>test string</t>
   </si>
   <si>
-    <t>测试boolList</t>
-  </si>
-  <si>
-    <t>测试byteList</t>
-  </si>
-  <si>
-    <t>测试sbyteList</t>
-  </si>
-  <si>
-    <t>测试shortList</t>
-  </si>
-  <si>
-    <t>测试ushortList</t>
-  </si>
-  <si>
-    <t>测试intList</t>
-  </si>
-  <si>
-    <t>测试uintList</t>
-  </si>
-  <si>
-    <t>测试longList</t>
-  </si>
-  <si>
-    <t>测试ulongList</t>
-  </si>
-  <si>
-    <t>测试floatList</t>
-  </si>
-  <si>
-    <t>测试doubleList</t>
-  </si>
-  <si>
-    <t>测试decimalList</t>
-  </si>
-  <si>
-    <t>测试stringList</t>
+    <t>测试booleanArray</t>
+  </si>
+  <si>
+    <t>测试byteArray</t>
+  </si>
+  <si>
+    <t>测试sbyteArray</t>
+  </si>
+  <si>
+    <t>测试shortArray</t>
+  </si>
+  <si>
+    <t>测试ushortArray</t>
+  </si>
+  <si>
+    <t>测试intArray</t>
+  </si>
+  <si>
+    <t>测试uintArray</t>
+  </si>
+  <si>
+    <t>测试longArray</t>
+  </si>
+  <si>
+    <t>测试ulongArray</t>
+  </si>
+  <si>
+    <t>测试floatArray</t>
+  </si>
+  <si>
+    <t>测试doubleArray</t>
+  </si>
+  <si>
+    <t>测试decimalArray</t>
+  </si>
+  <si>
+    <t>测试stringArray</t>
   </si>
   <si>
     <t>dsaweq你好！@#￥%……&amp;*（）</t>
@@ -326,10 +326,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -358,6 +358,73 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -366,25 +433,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -396,20 +471,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -427,76 +488,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -516,187 +516,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,6 +707,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -725,11 +734,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -749,17 +790,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -772,41 +807,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -815,10 +815,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -827,137 +827,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -971,6 +971,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="7" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -1034,6 +1037,7 @@
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -1368,8 +1372,8 @@
   <sheetPr/>
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z13" sqref="Z13"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="20" customHeight="1" outlineLevelRow="5"/>
@@ -1669,7 +1673,7 @@
       <c r="Q4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="8" t="s">
         <v>83</v>
       </c>
       <c r="S4" s="1" t="s">
@@ -1693,7 +1697,7 @@
       <c r="Y4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Z4" s="6" t="s">
+      <c r="Z4" s="7" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1719,7 +1723,7 @@
       <c r="K5" s="1">
         <v>-10.0214510024561</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="6">
         <v>9.99999999999999e+27</v>
       </c>
       <c r="M5" s="1" t="s">

</xml_diff>

<commit_message>
Add extension methods for type String.
</commit_message>
<xml_diff>
--- a/Data/TestData.xlsx
+++ b/Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13050"/>
+    <workbookView windowWidth="28080" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105">
   <si>
     <t>id</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>testString</t>
+  </si>
+  <si>
+    <t>testVector2</t>
+  </si>
+  <si>
+    <t>testVector3</t>
+  </si>
+  <si>
+    <t>testQuaternion</t>
   </si>
   <si>
     <t>testBooleanArray</t>
@@ -214,6 +223,15 @@
     <t>test string</t>
   </si>
   <si>
+    <t>测试Vector2</t>
+  </si>
+  <si>
+    <t>测试Vector3</t>
+  </si>
+  <si>
+    <t>测试Quaternion</t>
+  </si>
+  <si>
     <t>测试booleanArray</t>
   </si>
   <si>
@@ -254,6 +272,15 @@
   </si>
   <si>
     <t>dsaweq你好！@#￥%……&amp;*（）</t>
+  </si>
+  <si>
+    <t>(1, 2)</t>
+  </si>
+  <si>
+    <t>(1, 2, 3)</t>
+  </si>
+  <si>
+    <t>(1, 2, 3, 4)</t>
   </si>
   <si>
     <t>TRUE|false|0|1</t>
@@ -320,17 +347,26 @@
   <si>
     <t>!@#$%^&amp;*()_+QWERASDzxcv</t>
   </si>
+  <si>
+    <t>(0.1, 0.2)</t>
+  </si>
+  <si>
+    <t>(0.1, 0.2, 0.3)</t>
+  </si>
+  <si>
+    <t>(0.1, 0.2, 0.3, 0.4)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="7" formatCode="&quot;￥&quot;#,##0.00;&quot;￥&quot;\-#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -352,14 +388,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -381,7 +417,114 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -395,113 +538,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="BatangChe"/>
       <charset val="134"/>
@@ -516,187 +552,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,36 +751,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -771,6 +777,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -807,6 +828,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -815,10 +851,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -827,133 +863,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1370,10 +1406,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:AC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="20" customHeight="1" outlineLevelRow="5"/>
@@ -1381,7 +1419,7 @@
     <col min="1" max="16384" width="20.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:26">
+    <row r="1" customHeight="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1460,52 +1498,61 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" customHeight="1" spans="1:26">
+    <row r="2" customHeight="1" spans="1:29">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>41</v>
@@ -1540,88 +1587,106 @@
       <c r="Z2" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="AA2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="3" customHeight="1" spans="1:26">
+    <row r="3" customHeight="1" spans="1:29">
       <c r="A3" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
-    <row r="4" customHeight="1" spans="1:26">
+    <row r="4" customHeight="1" spans="1:29">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1659,49 +1724,58 @@
         <v>9.99999999999999e+27</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>83</v>
+        <v>88</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z4" s="7" t="s">
-        <v>91</v>
+        <v>96</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC4" s="7" t="s">
+        <v>100</v>
       </c>
     </row>
-    <row r="5" customHeight="1" spans="1:13">
+    <row r="5" customHeight="1" spans="1:16">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1727,7 +1801,16 @@
         <v>9.99999999999999e+27</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>92</v>
+        <v>101</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">

</xml_diff>